<commit_message>
implemented ebscore v2.0 with outsourced script files
</commit_message>
<xml_diff>
--- a/info/candidates.xlsx
+++ b/info/candidates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinscience/Dropbox/Icke/Work/somVar/info/candidates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahtin/mount/snakes/develop/somVarWES/info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC5B345-DB35-2945-9FB4-2F046945CE67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730DB8A4-3890-0145-AE6C-307F8663DE76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DLBCL" sheetId="1" r:id="rId1"/>
@@ -2467,8 +2467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E333"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8937,7 +8937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B387"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+    <sheetView topLeftCell="A372" workbookViewId="0">
       <selection activeCell="K87" sqref="K87"/>
     </sheetView>
   </sheetViews>

</xml_diff>